<commit_message>
optimiseringar parser. nu 5 min och inga icke schemalagda pass i DB
</commit_message>
<xml_diff>
--- a/WebApplication1/Schema.xlsx
+++ b/WebApplication1/Schema.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="4860" windowWidth="28800" windowHeight="12300" tabRatio="605"/>
+    <workbookView xWindow="0" yWindow="4860" windowWidth="28800" windowHeight="12300" tabRatio="605"/>
   </bookViews>
   <sheets>
     <sheet name="Schema1" sheetId="7" r:id="rId1"/>
@@ -1981,7 +1981,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6654" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6653" uniqueCount="91">
   <si>
     <t>Ejvergård</t>
   </si>
@@ -2269,16 +2269,10 @@
     <t>Sadeghi Arash</t>
   </si>
   <si>
-    <t>?</t>
-  </si>
-  <si>
     <t>Jonsson M</t>
   </si>
   <si>
     <t>Säfström</t>
-  </si>
-  <si>
-    <t>10</t>
   </si>
   <si>
     <t>R Lindqvist</t>
@@ -3876,9 +3870,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:QJ86"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="AL3" sqref="AL3"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="DG1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="FV50" sqref="FV50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9769,22 +9763,22 @@
     </row>
     <row r="5" spans="1:452" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B5" s="27" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="C5" s="25" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="D5" s="25" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="E5" s="25" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F5" s="25" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G5" s="25"/>
       <c r="H5" s="25"/>
@@ -12565,7 +12559,7 @@
     </row>
     <row r="8" spans="1:452" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B8" s="26" t="s">
         <v>25</v>
@@ -13491,7 +13485,7 @@
     </row>
     <row r="9" spans="1:452" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B9" s="26"/>
       <c r="C9" s="26"/>
@@ -17656,7 +17650,7 @@
     </row>
     <row r="14" spans="1:452" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B14" s="26" t="s">
         <v>30</v>
@@ -20447,7 +20441,7 @@
     </row>
     <row r="17" spans="1:452" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B17" s="8"/>
       <c r="C17" s="8"/>
@@ -21837,7 +21831,7 @@
     </row>
     <row r="19" spans="1:452" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B19" s="8"/>
       <c r="C19" s="8"/>
@@ -24733,7 +24727,7 @@
     </row>
     <row r="24" spans="1:452" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="6" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B24" s="8"/>
       <c r="C24" s="26"/>
@@ -26611,7 +26605,7 @@
     </row>
     <row r="27" spans="1:452" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="6" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B27" s="26"/>
       <c r="C27" s="8" t="s">
@@ -27359,9 +27353,7 @@
       <c r="EC28" s="8"/>
       <c r="ED28" s="8"/>
       <c r="EE28" s="8"/>
-      <c r="EF28" s="8" t="s">
-        <v>80</v>
-      </c>
+      <c r="EF28" s="8"/>
       <c r="EG28" s="8"/>
       <c r="EH28" s="8"/>
       <c r="EI28" s="8"/>
@@ -28273,7 +28265,7 @@
     </row>
     <row r="30" spans="1:452" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="6" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B30" s="8"/>
       <c r="C30" s="8"/>
@@ -30544,7 +30536,7 @@
     </row>
     <row r="35" spans="1:452" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="23" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B35" s="26" t="s">
         <v>36</v>
@@ -34042,7 +34034,7 @@
     </row>
     <row r="38" spans="1:452" s="5" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="23" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B38" s="26" t="s">
         <v>31</v>
@@ -35620,7 +35612,7 @@
       <c r="FO39" s="8"/>
       <c r="FP39" s="8"/>
       <c r="FQ39" s="8" t="s">
-        <v>83</v>
+        <v>34</v>
       </c>
       <c r="FR39" s="8" t="s">
         <v>27</v>

</xml_diff>

<commit_message>
Added groups to people and filtering on groups. Added sorting on groups and names to the table
</commit_message>
<xml_diff>
--- a/WebApplication1/Schema.xlsx
+++ b/WebApplication1/Schema.xlsx
@@ -1981,7 +1981,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6653" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6652" uniqueCount="91">
   <si>
     <t>Ejvergård</t>
   </si>
@@ -2257,9 +2257,6 @@
     <t>4sf</t>
   </si>
   <si>
-    <t>Jonsson M</t>
-  </si>
-  <si>
     <t>Säfström</t>
   </si>
   <si>
@@ -2300,6 +2297,9 @@
   </si>
   <si>
     <t>DNilsson</t>
+  </si>
+  <si>
+    <t>Jonsson</t>
   </si>
 </sst>
 </file>
@@ -3870,9 +3870,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:QJ86"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="A36" sqref="A36"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="FJ1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="GM30" sqref="GM30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9485,9 +9485,7 @@
       <c r="FU4" s="7"/>
       <c r="FV4" s="7"/>
       <c r="FW4" s="7"/>
-      <c r="FX4" s="7" t="s">
-        <v>67</v>
-      </c>
+      <c r="FX4" s="7"/>
       <c r="FY4" s="7"/>
       <c r="FZ4" s="7"/>
       <c r="GA4" s="7"/>
@@ -9763,7 +9761,7 @@
     </row>
     <row r="5" spans="1:452" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B5" s="27" t="s">
         <v>27</v>
@@ -12559,7 +12557,7 @@
     </row>
     <row r="8" spans="1:452" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B8" s="26" t="s">
         <v>25</v>
@@ -13485,7 +13483,7 @@
     </row>
     <row r="9" spans="1:452" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B9" s="26"/>
       <c r="C9" s="26"/>
@@ -17650,7 +17648,7 @@
     </row>
     <row r="14" spans="1:452" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B14" s="26" t="s">
         <v>30</v>
@@ -20441,7 +20439,7 @@
     </row>
     <row r="17" spans="1:452" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B17" s="8"/>
       <c r="C17" s="8"/>
@@ -21831,7 +21829,7 @@
     </row>
     <row r="19" spans="1:452" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B19" s="8"/>
       <c r="C19" s="8"/>
@@ -22381,7 +22379,7 @@
     </row>
     <row r="20" spans="1:452" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B20" s="8"/>
       <c r="C20" s="8"/>
@@ -22967,7 +22965,7 @@
     </row>
     <row r="21" spans="1:452" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B21" s="8"/>
       <c r="C21" s="26"/>
@@ -23547,7 +23545,7 @@
     </row>
     <row r="22" spans="1:452" s="5" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B22" s="8"/>
       <c r="C22" s="26"/>
@@ -24727,7 +24725,7 @@
     </row>
     <row r="24" spans="1:452" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="6" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B24" s="8"/>
       <c r="C24" s="26"/>
@@ -26605,7 +26603,7 @@
     </row>
     <row r="27" spans="1:452" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="6" t="s">
-        <v>76</v>
+        <v>90</v>
       </c>
       <c r="B27" s="26"/>
       <c r="C27" s="8" t="s">
@@ -28265,7 +28263,7 @@
     </row>
     <row r="30" spans="1:452" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="6" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B30" s="8"/>
       <c r="C30" s="8"/>
@@ -30536,7 +30534,7 @@
     </row>
     <row r="35" spans="1:452" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="23" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B35" s="26" t="s">
         <v>36</v>
@@ -31710,7 +31708,7 @@
     </row>
     <row r="36" spans="1:452" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="23" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B36" s="26" t="s">
         <v>33</v>
@@ -34034,7 +34032,7 @@
     </row>
     <row r="38" spans="1:452" s="5" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="23" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B38" s="26" t="s">
         <v>31</v>

</xml_diff>